<commit_message>
inserção DOC dados parciais
primeiro doc com analises parciais mas com documento formatado no layout final do trabalho em construção
</commit_message>
<xml_diff>
--- a/data/used_doc_files/Dados TCC/whr_all_years.xlsx
+++ b/data/used_doc_files/Dados TCC/whr_all_years.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Documents\GitHub\Projetos\TCC\TCC\data\used_doc_files\Dados TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91885497-99CA-4891-93C2-7954414E858D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE5015D-DCE5-4001-9BC9-5BD8D40C3035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_data" sheetId="1" r:id="rId1"/>
@@ -502,9 +502,6 @@
     <t>lowerwhisker</t>
   </si>
   <si>
-    <t>Explained by: Log GDP per capita</t>
-  </si>
-  <si>
     <t>Explained by: Social support</t>
   </si>
   <si>
@@ -536,6 +533,9 @@
   </si>
   <si>
     <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Explained by: Log GDP</t>
   </si>
 </sst>
 </file>
@@ -904,7 +904,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -927,10 +927,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>137</v>
@@ -947,26 +947,26 @@
       <c r="G1" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -3177,7 +3177,7 @@
         <v>2020</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>146</v>
@@ -4277,7 +4277,7 @@
         <v>2020</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>145</v>
@@ -6345,7 +6345,7 @@
         <v>2020</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>146</v>
@@ -9425,7 +9425,7 @@
         <v>2019</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>146</v>
@@ -10525,7 +10525,7 @@
         <v>2019</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D219" s="2" t="s">
         <v>145</v>
@@ -12593,7 +12593,7 @@
         <v>2019</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D266" s="2" t="s">
         <v>146</v>
@@ -15673,7 +15673,7 @@
         <v>2018</v>
       </c>
       <c r="C336" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D336" s="7" t="s">
         <v>146</v>
@@ -16773,7 +16773,7 @@
         <v>2018</v>
       </c>
       <c r="C361" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D361" s="7" t="s">
         <v>145</v>
@@ -18841,7 +18841,7 @@
         <v>2018</v>
       </c>
       <c r="C408" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D408" s="7" t="s">
         <v>146</v>
@@ -21921,7 +21921,7 @@
         <v>2017</v>
       </c>
       <c r="C478" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D478" s="7" t="s">
         <v>146</v>
@@ -23021,7 +23021,7 @@
         <v>2017</v>
       </c>
       <c r="C503" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D503" s="7" t="s">
         <v>145</v>
@@ -25089,7 +25089,7 @@
         <v>2017</v>
       </c>
       <c r="C550" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D550" s="7" t="s">
         <v>146</v>
@@ -28169,7 +28169,7 @@
         <v>2016</v>
       </c>
       <c r="C620" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D620" s="7" t="s">
         <v>146</v>
@@ -29269,7 +29269,7 @@
         <v>2016</v>
       </c>
       <c r="C645" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D645" s="7" t="s">
         <v>145</v>
@@ -31337,7 +31337,7 @@
         <v>2016</v>
       </c>
       <c r="C692" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D692" s="7" t="s">
         <v>146</v>
@@ -34417,7 +34417,7 @@
         <v>2015</v>
       </c>
       <c r="C762" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D762" s="7" t="s">
         <v>146</v>
@@ -35517,7 +35517,7 @@
         <v>2015</v>
       </c>
       <c r="C787" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D787" s="7" t="s">
         <v>145</v>
@@ -37585,7 +37585,7 @@
         <v>2015</v>
       </c>
       <c r="C834" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D834" s="7" t="s">
         <v>146</v>

</xml_diff>